<commit_message>
Actualización de cromograma 01-06
</commit_message>
<xml_diff>
--- a/3-Linea-Bases/SCIP/Linea-Base-1/SCIP-CP.xlsx
+++ b/3-Linea-Bases/SCIP/Linea-Base-1/SCIP-CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ing. de Software\8 - Gestión de Configuración y Mantenimiento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D17CD22-1695-4E21-8A9B-712F8F0E2D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA68ED1-DD9C-4ABD-AE36-598D1602D45C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B688ADBF-7033-4F25-B77C-86C1BC07C039}"/>
   </bookViews>
@@ -1048,32 +1048,6 @@
       <right style="thin">
         <color rgb="FFB1BBCC"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFB1BBCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB1BBCC"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFB1BBCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB1BBCC"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB1BBCC"/>
-      </right>
       <top style="thin">
         <color rgb="FFB1BBCC"/>
       </top>
@@ -1318,17 +1292,6 @@
       <right style="thin">
         <color rgb="FFB1BBCC"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFB1BBCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFB1BBCC"/>
-      </right>
       <top style="thin">
         <color rgb="FFB1BBCC"/>
       </top>
@@ -1348,12 +1311,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB1BBCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB1BBCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB1BBCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB1BBCC"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB1BBCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB1BBCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB1BBCC"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1403,21 +1411,6 @@
     <xf numFmtId="9" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1433,19 +1426,19 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1454,6 +1447,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1461,90 +1460,93 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="31" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1864,8 +1866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A3B3B80-6AC9-4507-B19B-F46B6EBD1C86}">
   <dimension ref="B1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1886,146 +1888,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="43" t="s">
         <v>171</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="52"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="45"/>
     </row>
     <row r="2" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="41" t="s">
         <v>151</v>
       </c>
-      <c r="F3" s="49"/>
+      <c r="F3" s="42"/>
     </row>
     <row r="4" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="E4" s="56">
+      <c r="E4" s="49">
         <v>4</v>
       </c>
-      <c r="F4" s="57"/>
+      <c r="F4" s="50"/>
     </row>
     <row r="5" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="E5" s="63" t="s">
+      <c r="E5" s="56" t="s">
         <v>247</v>
       </c>
-      <c r="F5" s="64"/>
+      <c r="F5" s="57"/>
     </row>
     <row r="6" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="E6" s="62" t="s">
+      <c r="E6" s="55" t="s">
         <v>150</v>
       </c>
-      <c r="F6" s="61"/>
+      <c r="F6" s="54"/>
     </row>
     <row r="7" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="E7" s="60">
+      <c r="E7" s="53">
         <v>45019</v>
       </c>
-      <c r="F7" s="61"/>
+      <c r="F7" s="54"/>
     </row>
     <row r="8" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="E8" s="58">
+      <c r="E8" s="51">
         <v>45107</v>
       </c>
-      <c r="F8" s="59"/>
+      <c r="F8" s="52"/>
     </row>
     <row r="9" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="30"/>
-      <c r="C10" s="31" t="s">
+      <c r="B10" s="25"/>
+      <c r="C10" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="31" t="s">
+      <c r="G10" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="30" t="s">
+      <c r="I10" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="J10" s="31" t="s">
+      <c r="J10" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="K10" s="30" t="s">
+      <c r="K10" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="L10" s="31" t="s">
+      <c r="L10" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="M10" s="30" t="s">
+      <c r="M10" s="25" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="C11" s="42">
+      <c r="C11" s="37">
         <v>1</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="25">
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="20">
         <v>1</v>
       </c>
-      <c r="M11" s="26" t="s">
+      <c r="M11" s="21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="54"/>
-      <c r="C12" s="43">
+      <c r="B12" s="47"/>
+      <c r="C12" s="38">
         <v>1.1000000000000001</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -2060,8 +2062,8 @@
       </c>
     </row>
     <row r="13" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="54"/>
-      <c r="C13" s="43">
+      <c r="B13" s="47"/>
+      <c r="C13" s="38">
         <v>1.2</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -2096,8 +2098,8 @@
       </c>
     </row>
     <row r="14" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="54"/>
-      <c r="C14" s="43">
+      <c r="B14" s="47"/>
+      <c r="C14" s="38">
         <v>1.3</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -2132,8 +2134,8 @@
       </c>
     </row>
     <row r="15" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="54"/>
-      <c r="C15" s="44">
+      <c r="B15" s="47"/>
+      <c r="C15" s="39">
         <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -2160,8 +2162,8 @@
       </c>
     </row>
     <row r="16" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="54"/>
-      <c r="C16" s="43">
+      <c r="B16" s="47"/>
+      <c r="C16" s="38">
         <v>2.1</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -2196,8 +2198,8 @@
       </c>
     </row>
     <row r="17" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="54"/>
-      <c r="C17" s="43" t="s">
+      <c r="B17" s="47"/>
+      <c r="C17" s="38" t="s">
         <v>88</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -2232,8 +2234,8 @@
       </c>
     </row>
     <row r="18" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="54"/>
-      <c r="C18" s="43" t="s">
+      <c r="B18" s="47"/>
+      <c r="C18" s="38" t="s">
         <v>89</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -2268,8 +2270,8 @@
       </c>
     </row>
     <row r="19" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="54"/>
-      <c r="C19" s="43" t="s">
+      <c r="B19" s="47"/>
+      <c r="C19" s="38" t="s">
         <v>90</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -2304,8 +2306,8 @@
       </c>
     </row>
     <row r="20" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="54"/>
-      <c r="C20" s="43" t="s">
+      <c r="B20" s="47"/>
+      <c r="C20" s="38" t="s">
         <v>91</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -2340,8 +2342,8 @@
       </c>
     </row>
     <row r="21" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="54"/>
-      <c r="C21" s="43" t="s">
+      <c r="B21" s="47"/>
+      <c r="C21" s="38" t="s">
         <v>92</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -2376,8 +2378,8 @@
       </c>
     </row>
     <row r="22" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="54"/>
-      <c r="C22" s="43" t="s">
+      <c r="B22" s="47"/>
+      <c r="C22" s="38" t="s">
         <v>93</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -2412,8 +2414,8 @@
       </c>
     </row>
     <row r="23" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="54"/>
-      <c r="C23" s="43" t="s">
+      <c r="B23" s="47"/>
+      <c r="C23" s="38" t="s">
         <v>94</v>
       </c>
       <c r="D23" s="5" t="s">
@@ -2448,8 +2450,8 @@
       </c>
     </row>
     <row r="24" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="54"/>
-      <c r="C24" s="43" t="s">
+      <c r="B24" s="47"/>
+      <c r="C24" s="38" t="s">
         <v>95</v>
       </c>
       <c r="D24" s="5" t="s">
@@ -2484,8 +2486,8 @@
       </c>
     </row>
     <row r="25" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="54"/>
-      <c r="C25" s="43" t="s">
+      <c r="B25" s="47"/>
+      <c r="C25" s="38" t="s">
         <v>96</v>
       </c>
       <c r="D25" s="5" t="s">
@@ -2520,8 +2522,8 @@
       </c>
     </row>
     <row r="26" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="54"/>
-      <c r="C26" s="43">
+      <c r="B26" s="47"/>
+      <c r="C26" s="38">
         <v>2.2000000000000002</v>
       </c>
       <c r="D26" s="5" t="s">
@@ -2556,8 +2558,8 @@
       </c>
     </row>
     <row r="27" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="54"/>
-      <c r="C27" s="43">
+      <c r="B27" s="47"/>
+      <c r="C27" s="38">
         <v>2.2999999999999998</v>
       </c>
       <c r="D27" s="5" t="s">
@@ -2592,8 +2594,8 @@
       </c>
     </row>
     <row r="28" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="54"/>
-      <c r="C28" s="43">
+      <c r="B28" s="47"/>
+      <c r="C28" s="38">
         <v>2.4</v>
       </c>
       <c r="D28" s="5" t="s">
@@ -2628,8 +2630,8 @@
       </c>
     </row>
     <row r="29" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="54"/>
-      <c r="C29" s="43">
+      <c r="B29" s="47"/>
+      <c r="C29" s="38">
         <v>2.5</v>
       </c>
       <c r="D29" s="5" t="s">
@@ -2664,8 +2666,8 @@
       </c>
     </row>
     <row r="30" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="54"/>
-      <c r="C30" s="43">
+      <c r="B30" s="47"/>
+      <c r="C30" s="38">
         <v>2.6</v>
       </c>
       <c r="D30" s="5" t="s">
@@ -2700,8 +2702,8 @@
       </c>
     </row>
     <row r="31" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="54"/>
-      <c r="C31" s="43">
+      <c r="B31" s="47"/>
+      <c r="C31" s="38">
         <v>2.7</v>
       </c>
       <c r="D31" s="5" t="s">
@@ -2736,8 +2738,8 @@
       </c>
     </row>
     <row r="32" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="54"/>
-      <c r="C32" s="43">
+      <c r="B32" s="47"/>
+      <c r="C32" s="38">
         <v>2.8</v>
       </c>
       <c r="D32" s="5" t="s">
@@ -2772,46 +2774,46 @@
       </c>
     </row>
     <row r="33" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="55"/>
-      <c r="C33" s="45">
+      <c r="B33" s="48"/>
+      <c r="C33" s="59">
         <v>2.9</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="G33" s="14" t="s">
+      <c r="G33" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="H33" s="14" t="s">
+      <c r="H33" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="I33" s="14" t="s">
+      <c r="I33" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="J33" s="14" t="s">
+      <c r="J33" s="22" t="s">
         <v>245</v>
       </c>
-      <c r="K33" s="14" t="s">
+      <c r="K33" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="L33" s="9">
+      <c r="L33" s="24">
         <v>1</v>
       </c>
-      <c r="M33" s="32" t="s">
+      <c r="M33" s="60" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="34" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="54" t="s">
+      <c r="B34" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="C34" s="46">
+      <c r="C34" s="61">
         <v>3</v>
       </c>
       <c r="D34" s="18" t="s">
@@ -2831,15 +2833,15 @@
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
       <c r="L34" s="20">
-        <v>0.74</v>
+        <v>0.9</v>
       </c>
       <c r="M34" s="21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="35" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="54"/>
-      <c r="C35" s="43">
+      <c r="B35" s="47"/>
+      <c r="C35" s="58">
         <v>3.1</v>
       </c>
       <c r="D35" s="5" t="s">
@@ -2874,8 +2876,8 @@
       </c>
     </row>
     <row r="36" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="54"/>
-      <c r="C36" s="43">
+      <c r="B36" s="47"/>
+      <c r="C36" s="58">
         <v>3.2</v>
       </c>
       <c r="D36" s="5" t="s">
@@ -2910,8 +2912,8 @@
       </c>
     </row>
     <row r="37" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="54"/>
-      <c r="C37" s="43">
+      <c r="B37" s="47"/>
+      <c r="C37" s="58">
         <v>3.3</v>
       </c>
       <c r="D37" s="5" t="s">
@@ -2946,8 +2948,8 @@
       </c>
     </row>
     <row r="38" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="54"/>
-      <c r="C38" s="43">
+      <c r="B38" s="47"/>
+      <c r="C38" s="58">
         <v>3.4</v>
       </c>
       <c r="D38" s="5" t="s">
@@ -2982,8 +2984,8 @@
       </c>
     </row>
     <row r="39" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="54"/>
-      <c r="C39" s="43">
+      <c r="B39" s="47"/>
+      <c r="C39" s="58">
         <v>3.5</v>
       </c>
       <c r="D39" s="5" t="s">
@@ -3018,8 +3020,8 @@
       </c>
     </row>
     <row r="40" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="54"/>
-      <c r="C40" s="43">
+      <c r="B40" s="47"/>
+      <c r="C40" s="58">
         <v>3.6</v>
       </c>
       <c r="D40" s="5" t="s">
@@ -3054,8 +3056,8 @@
       </c>
     </row>
     <row r="41" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="54"/>
-      <c r="C41" s="43">
+      <c r="B41" s="47"/>
+      <c r="C41" s="58">
         <v>3.7</v>
       </c>
       <c r="D41" s="5" t="s">
@@ -3090,8 +3092,8 @@
       </c>
     </row>
     <row r="42" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="54"/>
-      <c r="C42" s="43">
+      <c r="B42" s="47"/>
+      <c r="C42" s="58">
         <v>3.8</v>
       </c>
       <c r="D42" s="5" t="s">
@@ -3119,15 +3121,15 @@
         <v>221</v>
       </c>
       <c r="L42" s="9">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="M42" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="43" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="54"/>
-      <c r="C43" s="43">
+      <c r="B43" s="47"/>
+      <c r="C43" s="58">
         <v>3.9</v>
       </c>
       <c r="D43" s="5" t="s">
@@ -3155,81 +3157,81 @@
         <v>222</v>
       </c>
       <c r="L43" s="9">
+        <v>1</v>
+      </c>
+      <c r="M43" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="47"/>
+      <c r="C44" s="62" t="s">
+        <v>144</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H44" s="14">
+        <v>3.9</v>
+      </c>
+      <c r="I44" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J44" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="K44" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="L44" s="16">
         <v>0</v>
       </c>
-      <c r="M43" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="54"/>
-      <c r="C44" s="47" t="s">
-        <v>144</v>
-      </c>
-      <c r="D44" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="E44" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="F44" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="G44" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="H44" s="27">
-        <v>3.9</v>
-      </c>
-      <c r="I44" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="J44" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="K44" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="L44" s="29">
+      <c r="M44" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="C45" s="37">
+        <v>4</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="G45" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="20">
         <v>0</v>
       </c>
-      <c r="M44" s="32" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="53" t="s">
-        <v>134</v>
-      </c>
-      <c r="C45" s="42">
-        <v>4</v>
-      </c>
-      <c r="D45" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="E45" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="F45" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="G45" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="H45" s="24"/>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="24"/>
-      <c r="L45" s="25">
-        <v>0</v>
-      </c>
-      <c r="M45" s="26" t="s">
+      <c r="M45" s="21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="46" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="54"/>
-      <c r="C46" s="43">
+      <c r="B46" s="47"/>
+      <c r="C46" s="38">
         <v>4.0999999999999996</v>
       </c>
       <c r="D46" s="5" t="s">
@@ -3264,8 +3266,8 @@
       </c>
     </row>
     <row r="47" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="54"/>
-      <c r="C47" s="43">
+      <c r="B47" s="47"/>
+      <c r="C47" s="38">
         <v>4.2</v>
       </c>
       <c r="D47" s="5" t="s">
@@ -3300,8 +3302,8 @@
       </c>
     </row>
     <row r="48" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="54"/>
-      <c r="C48" s="43">
+      <c r="B48" s="47"/>
+      <c r="C48" s="38">
         <v>4.3</v>
       </c>
       <c r="D48" s="5" t="s">
@@ -3336,8 +3338,8 @@
       </c>
     </row>
     <row r="49" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="54"/>
-      <c r="C49" s="43">
+      <c r="B49" s="47"/>
+      <c r="C49" s="38">
         <v>4.4000000000000004</v>
       </c>
       <c r="D49" s="5" t="s">
@@ -3372,8 +3374,8 @@
       </c>
     </row>
     <row r="50" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="55"/>
-      <c r="C50" s="45">
+      <c r="B50" s="48"/>
+      <c r="C50" s="40">
         <v>4.5</v>
       </c>
       <c r="D50" s="15" t="s">
@@ -3394,7 +3396,7 @@
       <c r="I50" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="J50" s="40" t="s">
+      <c r="J50" s="35" t="s">
         <v>98</v>
       </c>
       <c r="K50" s="14" t="s">
@@ -3403,16 +3405,16 @@
       <c r="L50" s="16">
         <v>0</v>
       </c>
-      <c r="M50" s="32" t="s">
+      <c r="M50" s="27" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="51" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="52" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I52" s="41" t="s">
+      <c r="I52" s="36" t="s">
         <v>259</v>
       </c>
-      <c r="J52" s="41" t="s">
+      <c r="J52" s="36" t="s">
         <v>249</v>
       </c>
     </row>
@@ -3451,120 +3453,120 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.42578125" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="33"/>
-    <col min="2" max="2" width="41.7109375" style="33" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" style="33" customWidth="1"/>
-    <col min="4" max="16384" width="18.42578125" style="33"/>
+    <col min="1" max="1" width="18.42578125" style="28"/>
+    <col min="2" max="2" width="41.7109375" style="28" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" style="28" customWidth="1"/>
+    <col min="4" max="16384" width="18.42578125" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="27" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="30" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="29" t="s">
         <v>181</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="33" t="s">
         <v>190</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="30" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="30" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="29" t="s">
         <v>183</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="30" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="30" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="29" t="s">
         <v>185</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="30" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="30" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="29" t="s">
         <v>187</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="33" t="s">
         <v>196</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="30" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="31" t="s">
         <v>188</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="34" t="s">
         <v>196</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="32" t="s">
         <v>204</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización del cronograma 02-06
</commit_message>
<xml_diff>
--- a/3-Linea-Bases/SCIP/Linea-Base-1/SCIP-CP.xlsx
+++ b/3-Linea-Bases/SCIP/Linea-Base-1/SCIP-CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ing. de Software\8 - Gestión de Configuración y Mantenimiento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA68ED1-DD9C-4ABD-AE36-598D1602D45C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC3D9C3-4928-457B-ADB1-B1F33EB0899C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B688ADBF-7033-4F25-B77C-86C1BC07C039}"/>
   </bookViews>
@@ -1483,6 +1483,21 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="31" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1532,21 +1547,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="31" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1867,7 +1867,7 @@
   <dimension ref="B1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1888,75 +1888,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="45"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="50"/>
     </row>
     <row r="2" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="F3" s="42"/>
+      <c r="F3" s="47"/>
     </row>
     <row r="4" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="E4" s="49">
+      <c r="E4" s="54">
         <v>4</v>
       </c>
-      <c r="F4" s="50"/>
+      <c r="F4" s="55"/>
     </row>
     <row r="5" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="E5" s="56" t="s">
+      <c r="E5" s="61" t="s">
         <v>247</v>
       </c>
-      <c r="F5" s="57"/>
+      <c r="F5" s="62"/>
     </row>
     <row r="6" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="E6" s="55" t="s">
+      <c r="E6" s="60" t="s">
         <v>150</v>
       </c>
-      <c r="F6" s="54"/>
+      <c r="F6" s="59"/>
     </row>
     <row r="7" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="E7" s="53">
+      <c r="E7" s="58">
         <v>45019</v>
       </c>
-      <c r="F7" s="54"/>
+      <c r="F7" s="59"/>
     </row>
     <row r="8" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="E8" s="51">
+      <c r="E8" s="56">
         <v>45107</v>
       </c>
-      <c r="F8" s="52"/>
+      <c r="F8" s="57"/>
     </row>
     <row r="9" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1996,7 +1996,7 @@
       </c>
     </row>
     <row r="11" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="51" t="s">
         <v>132</v>
       </c>
       <c r="C11" s="37">
@@ -2026,7 +2026,7 @@
       </c>
     </row>
     <row r="12" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="47"/>
+      <c r="B12" s="52"/>
       <c r="C12" s="38">
         <v>1.1000000000000001</v>
       </c>
@@ -2062,7 +2062,7 @@
       </c>
     </row>
     <row r="13" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="47"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="38">
         <v>1.2</v>
       </c>
@@ -2098,7 +2098,7 @@
       </c>
     </row>
     <row r="14" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="47"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="38">
         <v>1.3</v>
       </c>
@@ -2134,7 +2134,7 @@
       </c>
     </row>
     <row r="15" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="47"/>
+      <c r="B15" s="52"/>
       <c r="C15" s="39">
         <v>2</v>
       </c>
@@ -2162,7 +2162,7 @@
       </c>
     </row>
     <row r="16" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="47"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="38">
         <v>2.1</v>
       </c>
@@ -2198,7 +2198,7 @@
       </c>
     </row>
     <row r="17" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="38" t="s">
         <v>88</v>
       </c>
@@ -2234,7 +2234,7 @@
       </c>
     </row>
     <row r="18" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="47"/>
+      <c r="B18" s="52"/>
       <c r="C18" s="38" t="s">
         <v>89</v>
       </c>
@@ -2270,7 +2270,7 @@
       </c>
     </row>
     <row r="19" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="47"/>
+      <c r="B19" s="52"/>
       <c r="C19" s="38" t="s">
         <v>90</v>
       </c>
@@ -2306,7 +2306,7 @@
       </c>
     </row>
     <row r="20" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="47"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="38" t="s">
         <v>91</v>
       </c>
@@ -2342,7 +2342,7 @@
       </c>
     </row>
     <row r="21" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="47"/>
+      <c r="B21" s="52"/>
       <c r="C21" s="38" t="s">
         <v>92</v>
       </c>
@@ -2378,7 +2378,7 @@
       </c>
     </row>
     <row r="22" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="47"/>
+      <c r="B22" s="52"/>
       <c r="C22" s="38" t="s">
         <v>93</v>
       </c>
@@ -2414,7 +2414,7 @@
       </c>
     </row>
     <row r="23" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="47"/>
+      <c r="B23" s="52"/>
       <c r="C23" s="38" t="s">
         <v>94</v>
       </c>
@@ -2450,7 +2450,7 @@
       </c>
     </row>
     <row r="24" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="47"/>
+      <c r="B24" s="52"/>
       <c r="C24" s="38" t="s">
         <v>95</v>
       </c>
@@ -2486,7 +2486,7 @@
       </c>
     </row>
     <row r="25" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="47"/>
+      <c r="B25" s="52"/>
       <c r="C25" s="38" t="s">
         <v>96</v>
       </c>
@@ -2522,7 +2522,7 @@
       </c>
     </row>
     <row r="26" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="47"/>
+      <c r="B26" s="52"/>
       <c r="C26" s="38">
         <v>2.2000000000000002</v>
       </c>
@@ -2558,7 +2558,7 @@
       </c>
     </row>
     <row r="27" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="47"/>
+      <c r="B27" s="52"/>
       <c r="C27" s="38">
         <v>2.2999999999999998</v>
       </c>
@@ -2594,7 +2594,7 @@
       </c>
     </row>
     <row r="28" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="47"/>
+      <c r="B28" s="52"/>
       <c r="C28" s="38">
         <v>2.4</v>
       </c>
@@ -2630,7 +2630,7 @@
       </c>
     </row>
     <row r="29" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="47"/>
+      <c r="B29" s="52"/>
       <c r="C29" s="38">
         <v>2.5</v>
       </c>
@@ -2666,7 +2666,7 @@
       </c>
     </row>
     <row r="30" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="47"/>
+      <c r="B30" s="52"/>
       <c r="C30" s="38">
         <v>2.6</v>
       </c>
@@ -2702,7 +2702,7 @@
       </c>
     </row>
     <row r="31" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="47"/>
+      <c r="B31" s="52"/>
       <c r="C31" s="38">
         <v>2.7</v>
       </c>
@@ -2738,7 +2738,7 @@
       </c>
     </row>
     <row r="32" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="47"/>
+      <c r="B32" s="52"/>
       <c r="C32" s="38">
         <v>2.8</v>
       </c>
@@ -2774,8 +2774,8 @@
       </c>
     </row>
     <row r="33" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="48"/>
-      <c r="C33" s="59">
+      <c r="B33" s="53"/>
+      <c r="C33" s="42">
         <v>2.9</v>
       </c>
       <c r="D33" s="23" t="s">
@@ -2805,15 +2805,15 @@
       <c r="L33" s="24">
         <v>1</v>
       </c>
-      <c r="M33" s="60" t="s">
+      <c r="M33" s="43" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="34" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="C34" s="61">
+      <c r="C34" s="44">
         <v>3</v>
       </c>
       <c r="D34" s="18" t="s">
@@ -2833,15 +2833,15 @@
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
       <c r="L34" s="20">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="M34" s="21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="35" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="47"/>
-      <c r="C35" s="58">
+      <c r="B35" s="52"/>
+      <c r="C35" s="41">
         <v>3.1</v>
       </c>
       <c r="D35" s="5" t="s">
@@ -2876,8 +2876,8 @@
       </c>
     </row>
     <row r="36" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="47"/>
-      <c r="C36" s="58">
+      <c r="B36" s="52"/>
+      <c r="C36" s="41">
         <v>3.2</v>
       </c>
       <c r="D36" s="5" t="s">
@@ -2912,8 +2912,8 @@
       </c>
     </row>
     <row r="37" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="47"/>
-      <c r="C37" s="58">
+      <c r="B37" s="52"/>
+      <c r="C37" s="41">
         <v>3.3</v>
       </c>
       <c r="D37" s="5" t="s">
@@ -2948,8 +2948,8 @@
       </c>
     </row>
     <row r="38" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="47"/>
-      <c r="C38" s="58">
+      <c r="B38" s="52"/>
+      <c r="C38" s="41">
         <v>3.4</v>
       </c>
       <c r="D38" s="5" t="s">
@@ -2984,8 +2984,8 @@
       </c>
     </row>
     <row r="39" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="47"/>
-      <c r="C39" s="58">
+      <c r="B39" s="52"/>
+      <c r="C39" s="41">
         <v>3.5</v>
       </c>
       <c r="D39" s="5" t="s">
@@ -3020,8 +3020,8 @@
       </c>
     </row>
     <row r="40" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="47"/>
-      <c r="C40" s="58">
+      <c r="B40" s="52"/>
+      <c r="C40" s="41">
         <v>3.6</v>
       </c>
       <c r="D40" s="5" t="s">
@@ -3056,8 +3056,8 @@
       </c>
     </row>
     <row r="41" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="47"/>
-      <c r="C41" s="58">
+      <c r="B41" s="52"/>
+      <c r="C41" s="41">
         <v>3.7</v>
       </c>
       <c r="D41" s="5" t="s">
@@ -3092,8 +3092,8 @@
       </c>
     </row>
     <row r="42" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="47"/>
-      <c r="C42" s="58">
+      <c r="B42" s="52"/>
+      <c r="C42" s="41">
         <v>3.8</v>
       </c>
       <c r="D42" s="5" t="s">
@@ -3128,8 +3128,8 @@
       </c>
     </row>
     <row r="43" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="47"/>
-      <c r="C43" s="58">
+      <c r="B43" s="52"/>
+      <c r="C43" s="41">
         <v>3.9</v>
       </c>
       <c r="D43" s="5" t="s">
@@ -3164,8 +3164,8 @@
       </c>
     </row>
     <row r="44" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="47"/>
-      <c r="C44" s="62" t="s">
+      <c r="B44" s="52"/>
+      <c r="C44" s="45" t="s">
         <v>144</v>
       </c>
       <c r="D44" s="15" t="s">
@@ -3193,14 +3193,14 @@
         <v>127</v>
       </c>
       <c r="L44" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M44" s="27" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="45" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="51" t="s">
         <v>134</v>
       </c>
       <c r="C45" s="37">
@@ -3230,7 +3230,7 @@
       </c>
     </row>
     <row r="46" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="47"/>
+      <c r="B46" s="52"/>
       <c r="C46" s="38">
         <v>4.0999999999999996</v>
       </c>
@@ -3266,7 +3266,7 @@
       </c>
     </row>
     <row r="47" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="47"/>
+      <c r="B47" s="52"/>
       <c r="C47" s="38">
         <v>4.2</v>
       </c>
@@ -3302,7 +3302,7 @@
       </c>
     </row>
     <row r="48" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="47"/>
+      <c r="B48" s="52"/>
       <c r="C48" s="38">
         <v>4.3</v>
       </c>
@@ -3338,7 +3338,7 @@
       </c>
     </row>
     <row r="49" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="47"/>
+      <c r="B49" s="52"/>
       <c r="C49" s="38">
         <v>4.4000000000000004</v>
       </c>
@@ -3374,7 +3374,7 @@
       </c>
     </row>
     <row r="50" spans="2:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="48"/>
+      <c r="B50" s="53"/>
       <c r="C50" s="40">
         <v>4.5</v>
       </c>

</xml_diff>